<commit_message>
added test run for Logistic Regression with scaling
</commit_message>
<xml_diff>
--- a/modeling/modeling_tracker.xlsx
+++ b/modeling/modeling_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/Machine Learning II/ml2challenge/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7BBFC7-011D-E240-98E3-849D41FE3388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F615A9-CC16-CE4D-BCE6-D4735EC2B622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>hyperparameters</t>
   </si>
@@ -127,12 +127,18 @@
   </si>
   <si>
     <t>20230214_1921_test.csv</t>
+  </si>
+  <si>
+    <t>scaling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -169,13 +175,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -525,7 +532,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,7 +544,7 @@
     <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
@@ -617,144 +624,217 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="4">
+        <v>44971.897916666669</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="1"/>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added first naive tests and submissions with xgb and only standardization
</commit_message>
<xml_diff>
--- a/modeling/modeling_tracker.xlsx
+++ b/modeling/modeling_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/Machine Learning II/ml2challenge/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F615A9-CC16-CE4D-BCE6-D4735EC2B622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F54101-8DA2-ED42-BA24-CAE1C49B37BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
     <sheet name="Dropdowns" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>hyperparameters</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>scaling</t>
+  </si>
+  <si>
+    <t>{"model__colsample_bylevel": 0.3, "model__max_depth": 7}</t>
+  </si>
+  <si>
+    <t>20230214_2204_naive_xgb.csv</t>
+  </si>
+  <si>
+    <t>{"model__colsample_bylevel": 0.2, "model__min_child_weight": 50, "model__max_depth": 5}</t>
   </si>
 </sst>
 </file>
@@ -137,7 +146,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -182,7 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -211,8 +220,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}" name="Tabelle2" displayName="Tabelle2" ref="A1:K30" totalsRowShown="0">
-  <autoFilter ref="A1:K30" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}" name="Tabelle2" displayName="Tabelle2" ref="A1:K31" totalsRowShown="0">
+  <autoFilter ref="A1:K31" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{AE3501BC-A93F-A44E-91E9-C2C9630E4D3B}" name="Timestamp" dataDxfId="2">
       <calculatedColumnFormula>NOW()</calculatedColumnFormula>
@@ -529,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA64AB39-C08B-144A-A441-ED0863E84DF0}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,39 +657,140 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="4">
+        <v>44971.910416666666</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="1"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="4">
+        <v>44971.919444444444</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.996</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="H6" s="6"/>
+      <c r="A6" s="4">
+        <v>44971.920138888891</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.99099999999999999</v>
+      </c>
       <c r="I6" s="6"/>
+      <c r="J6">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="4">
+        <v>44971.930555555555</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C7" s="1"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="4">
+        <v>44971.931250000001</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="H8" s="6"/>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.86299999999999999</v>
+      </c>
       <c r="I8" s="6"/>
+      <c r="J8" s="6">
+        <v>0.50765000000000005</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
@@ -835,6 +945,13 @@
       <c r="C30" s="1"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -848,19 +965,19 @@
           <x14:formula1>
             <xm:f>Dropdowns!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B30</xm:sqref>
+          <xm:sqref>B2:B31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5314795F-EFA8-DC48-AEC4-309F78D8EA79}">
           <x14:formula1>
             <xm:f>Dropdowns!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K30</xm:sqref>
+          <xm:sqref>K2:K31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E773B72D-11B4-4543-9E3B-6D3AAA4F3477}">
           <x14:formula1>
             <xm:f>Dropdowns!$E$2:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D30</xm:sqref>
+          <xm:sqref>D2:D31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
added logreg as basline submission
</commit_message>
<xml_diff>
--- a/modeling/modeling_tracker.xlsx
+++ b/modeling/modeling_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/Machine Learning II/ml2challenge/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F54101-8DA2-ED42-BA24-CAE1C49B37BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3A3A4F-3450-4440-A2E2-168297D623C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>hyperparameters</t>
   </si>
@@ -541,7 +541,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -793,11 +793,29 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="4">
+        <v>44971.939583333333</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C9" s="1"/>
-      <c r="H9" s="6"/>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.70799999999999996</v>
+      </c>
       <c r="I9" s="6"/>
+      <c r="J9">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>

</xml_diff>

<commit_message>
added init catboost tests and submission
</commit_message>
<xml_diff>
--- a/modeling/modeling_tracker.xlsx
+++ b/modeling/modeling_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/Machine Learning II/ml2challenge/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3A3A4F-3450-4440-A2E2-168297D623C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4FC43A-00B0-8A40-8C97-194AD26B0D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t>hyperparameters</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>{"model__colsample_bylevel": 0.2, "model__min_child_weight": 50, "model__max_depth": 5}</t>
+  </si>
+  <si>
+    <t>euclidean_dist, linear_dist, mean_hillshade, morning_hillshade, mean_amenties, aspect_dir, climatic_zone, geologic_zone, soil_type, scaling</t>
+  </si>
+  <si>
+    <t>False, False, False, False, False, False, False, False, False</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -818,18 +824,59 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="4">
+        <v>44971.973611111112</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C10" s="1"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="4">
+        <v>44971.974999999999</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C11" s="1"/>
-      <c r="H11" s="6"/>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.95</v>
+      </c>
       <c r="I11" s="6"/>
+      <c r="J11">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>

</xml_diff>

<commit_message>
update of new results till 24/02/2023 14:11:00
</commit_message>
<xml_diff>
--- a/modeling/modeling_tracker.xlsx
+++ b/modeling/modeling_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/Machine Learning II/ml2challenge/modeling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianna/Documents/master/2022-2023/Machine_learning_2/ml2challenge/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4FC43A-00B0-8A40-8C97-194AD26B0D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103DC28E-06B7-3E44-AB6D-6603B72D1161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" activeTab="1" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
   <si>
     <t>hyperparameters</t>
   </si>
@@ -102,9 +102,6 @@
     <t>SVM</t>
   </si>
   <si>
-    <t>RF</t>
-  </si>
-  <si>
     <t>Example</t>
   </si>
   <si>
@@ -145,6 +142,66 @@
   </si>
   <si>
     <t>False, False, False, False, False, False, False, False, False</t>
+  </si>
+  <si>
+    <t>euclidean_dist, linear_dist, mean_hillshade, morning_hillshade, mean_amenties, aspect_dir, climatic_zone, geologic_zone, soil_type</t>
+  </si>
+  <si>
+    <t>0.899</t>
+  </si>
+  <si>
+    <t>0.999</t>
+  </si>
+  <si>
+    <t>ExtraTrees</t>
+  </si>
+  <si>
+    <t>0.886</t>
+  </si>
+  <si>
+    <t>0.875</t>
+  </si>
+  <si>
+    <t>20230222_2147_naive_ExtraTrees</t>
+  </si>
+  <si>
+    <t>20230220_1616_xgb_try.csv</t>
+  </si>
+  <si>
+    <t>{'model__max_depth': None, 'model__max_features': 0.5, 'model__n_estimators': 100}</t>
+  </si>
+  <si>
+    <t>val accuracy: 0.903</t>
+  </si>
+  <si>
+    <t>20230222_2220_ExtraTrees_tuned.csv</t>
+  </si>
+  <si>
+    <t>{'model__max_depth': None, 'model__max_features': 0.6, 'model__n_estimators': 110}</t>
+  </si>
+  <si>
+    <t>val accuracy: 0.902</t>
+  </si>
+  <si>
+    <t>20230222_2301_ExtraTrees_tuned.csv</t>
+  </si>
+  <si>
+    <t>0.907</t>
+  </si>
+  <si>
+    <t>{'model__learning_rate': 0.2, 'model__max_depth': 10, 'model__n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>20230223_0851_XGB_tuned</t>
+  </si>
+  <si>
+    <t>{'model__colsample_bytree': 1.0, 'model__learning_rate': 0.2, 'model__max_depth': 10, 'model__n_estimators': 220, 'model__subsample': 1.0}</t>
+  </si>
+  <si>
+    <t>20230223_1000_XGB_tuned2</t>
+  </si>
+  <si>
+    <t>DecTree</t>
   </si>
 </sst>
 </file>
@@ -178,7 +235,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -186,23 +243,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
     </dxf>
@@ -211,6 +304,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -226,21 +322,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}" name="Tabelle2" displayName="Tabelle2" ref="A1:K31" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}" name="Tabelle2" displayName="Tabelle2" ref="A1:K31" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:K31" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{AE3501BC-A93F-A44E-91E9-C2C9630E4D3B}" name="Timestamp" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{AE3501BC-A93F-A44E-91E9-C2C9630E4D3B}" name="Timestamp" dataDxfId="5">
       <calculatedColumnFormula>NOW()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{15C54594-C213-1040-BB39-08AD944E191F}" name="Modeling Type" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{648BE996-BCA1-8A48-875C-7BB80DC12EAC}" name="Submission Name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{15C54594-C213-1040-BB39-08AD944E191F}" name="Modeling Type" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{648BE996-BCA1-8A48-875C-7BB80DC12EAC}" name="Submission Name" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{5E4B52D5-07C9-6748-9EFB-13CFB56CC836}" name="Model"/>
     <tableColumn id="4" xr3:uid="{0CA337F9-6EAC-2245-A0E9-1CC0549A66D2}" name="data_enigneering"/>
     <tableColumn id="5" xr3:uid="{E165C24C-21E3-7746-ADCA-4046945B8FF4}" name="drop_original"/>
     <tableColumn id="6" xr3:uid="{5F373FDA-F78B-A445-AECD-2FBF1D911CBF}" name="hyperparameters"/>
-    <tableColumn id="7" xr3:uid="{57B2801D-A688-2F4B-BD21-80E36348E592}" name="(Mean CV) Train Accuracy"/>
-    <tableColumn id="8" xr3:uid="{8A9A517A-9CA3-F94D-928C-325BD7B38657}" name="Mean CV Test Accuracy"/>
-    <tableColumn id="9" xr3:uid="{62E583F3-DEF1-184A-B39C-7DD9F304B3F5}" name="Kaggle Score"/>
+    <tableColumn id="7" xr3:uid="{57B2801D-A688-2F4B-BD21-80E36348E592}" name="(Mean CV) Train Accuracy" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{8A9A517A-9CA3-F94D-928C-325BD7B38657}" name="Mean CV Test Accuracy" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{62E583F3-DEF1-184A-B39C-7DD9F304B3F5}" name="Kaggle Score" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{2C5DD473-C08D-2248-8F07-9BB79E2E24F3}" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -248,7 +344,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -544,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA64AB39-C08B-144A-A441-ED0863E84DF0}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="108" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,48 +655,48 @@
     <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="H1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>44973.683333333334</v>
       </c>
@@ -608,37 +704,37 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="H2" s="7">
         <v>0.7</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="7">
         <v>0.7</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="7">
         <v>0.71</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>44971.897916666669</v>
       </c>
@@ -650,19 +746,19 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="6">
+        <v>29</v>
+      </c>
+      <c r="H3" s="8">
         <v>0.70899999999999996</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="8">
         <v>0.70199999999999996</v>
       </c>
       <c r="K3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>44971.910416666666</v>
       </c>
@@ -674,19 +770,19 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="6">
+        <v>29</v>
+      </c>
+      <c r="H4" s="8">
         <v>0.98899999999999999</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="8">
         <v>0.85699999999999998</v>
       </c>
       <c r="K4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>44971.919444444444</v>
       </c>
@@ -698,22 +794,22 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="H5" s="8">
         <v>0.996</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="8">
         <v>0.85599999999999998</v>
       </c>
       <c r="K5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>44971.920138888891</v>
       </c>
@@ -721,29 +817,29 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="H6" s="8">
         <v>0.99099999999999999</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6">
+      <c r="I6" s="8"/>
+      <c r="J6" s="6">
         <v>0.55600000000000005</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>44971.930555555555</v>
       </c>
@@ -755,22 +851,22 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="6">
+        <v>32</v>
+      </c>
+      <c r="H7" s="8">
         <v>0.86499999999999999</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="8">
         <v>0.80100000000000005</v>
       </c>
       <c r="K7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>44971.931250000001</v>
       </c>
@@ -782,23 +878,23 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="6">
+        <v>32</v>
+      </c>
+      <c r="H8" s="8">
         <v>0.86299999999999999</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6">
+      <c r="I8" s="8"/>
+      <c r="J8" s="8">
         <v>0.50765000000000005</v>
       </c>
       <c r="K8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>44971.939583333333</v>
       </c>
@@ -810,20 +906,20 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="6">
+        <v>29</v>
+      </c>
+      <c r="H9" s="8">
         <v>0.70799999999999996</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9">
+      <c r="I9" s="8"/>
+      <c r="J9" s="6">
         <v>0.42299999999999999</v>
       </c>
       <c r="K9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>44971.973611111112</v>
       </c>
@@ -835,22 +931,22 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="6">
+      <c r="H10" s="8">
         <v>0.95599999999999996</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="8">
         <v>0.86499999999999999</v>
       </c>
       <c r="K10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>44971.974999999999</v>
       </c>
@@ -862,161 +958,448 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
         <v>34</v>
       </c>
-      <c r="F11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="6">
+      <c r="H11" s="8">
         <v>0.95</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11">
+      <c r="I11" s="8"/>
+      <c r="J11" s="6">
         <v>0.55500000000000005</v>
       </c>
       <c r="K11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>44977.675694444442</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C12" s="1"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="1"/>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>44977.677777777775</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="6">
+        <v>0.81423999999999996</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>44979.9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C14" s="1"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1"/>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>44979.900694444441</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C15" s="1"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="1"/>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>44979.907638888886</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="8">
+        <v>1</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0.64946999999999999</v>
+      </c>
+      <c r="K16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>44979.915972222225</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C17" s="1"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1"/>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="K17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>44979.930555555555</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="8">
+        <v>1</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="6">
+        <v>0.82843999999999995</v>
+      </c>
+      <c r="K18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>44979.956944444442</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C19" s="1"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="K19" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>44979.959027777775</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1</v>
+      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="6">
+        <v>0.82972999999999997</v>
+      </c>
+      <c r="K20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>44979.969444444447</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C21" s="1"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="K21" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>44980.959027777775</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" s="8">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="6">
+        <v>0.83438000000000001</v>
+      </c>
+      <c r="K22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>44979.376388888886</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C23" s="1"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="1"/>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="K23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>44979.416666666664</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="8">
+        <v>1</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="6">
+        <v>0.83453999999999995</v>
+      </c>
+      <c r="K24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>44981.481944444444</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C25" s="1"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="1"/>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="8">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="K25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>44981.481944444444</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C26" s="1"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="8">
+        <v>1</v>
+      </c>
+      <c r="I26" s="6">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="K26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1052,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A561FA97-048C-B04D-9B19-9201C434118E}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1121,7 +1504,17 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>21</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of new results till 1/3/23 10:35
</commit_message>
<xml_diff>
--- a/modeling/modeling_tracker.xlsx
+++ b/modeling/modeling_tracker.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianna/Documents/master/2022-2023/Machine_learning_2/ml2challenge/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D2B4A9-56D5-E048-B58C-270A54EEC2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8CE6B6-9AB6-FC49-A186-A85462F76E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="98">
   <si>
     <t>hyperparameters</t>
   </si>
@@ -171,9 +171,6 @@
     <t>{'model__max_depth': None, 'model__max_features': 0.5, 'model__n_estimators': 100}</t>
   </si>
   <si>
-    <t>val accuracy: 0.903</t>
-  </si>
-  <si>
     <t>20230222_2220_ExtraTrees_tuned.csv</t>
   </si>
   <si>
@@ -217,16 +214,170 @@
   </si>
   <si>
     <t>0.902</t>
+  </si>
+  <si>
+    <t>20230228_1128_XGB_pca15</t>
+  </si>
+  <si>
+    <t>0.887</t>
+  </si>
+  <si>
+    <t>euclidean_dist, morning_hillshade</t>
+  </si>
+  <si>
+    <t>euclidean_dist, morning_hillshade, aspect_dir</t>
+  </si>
+  <si>
+    <t>True, True, True, False, False, False, False, False, False</t>
+  </si>
+  <si>
+    <t>False, False, True, False, False, False, False, False, False</t>
+  </si>
+  <si>
+    <t>euclidean_dist, morning_hillshade, aspec_dir</t>
+  </si>
+  <si>
+    <t>0.898</t>
+  </si>
+  <si>
+    <t>20230228_1241_XGB_feat_selection</t>
+  </si>
+  <si>
+    <t>{'model__colsample_bytree': 1.0, 'model__learning_rate': 0.2, 'model__max_depth': 10, 'model__min_child_weight': 1, 'model__n_estimators': 350, 'model__subsample': 1.0}</t>
+  </si>
+  <si>
+    <t>0.808</t>
+  </si>
+  <si>
+    <t>0.780</t>
+  </si>
+  <si>
+    <t>0.848</t>
+  </si>
+  <si>
+    <t>{'model__C': 100, 'model__degree': 2, 'model__gamma': 'scale', 'model__kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>0.952</t>
+  </si>
+  <si>
+    <t>0.847</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>{'model__criterion': 'entropy', 'model__max_depth': 50, 'model__max_features': 'sqrt', 'model__min_samples_leaf': 1, 'model__min_samples_split': 2}</t>
+  </si>
+  <si>
+    <t>0.791</t>
+  </si>
+  <si>
+    <t>0.796</t>
+  </si>
+  <si>
+    <t>{'model__criterion': 'entropy', 'model__max_depth': 100, 'model__max_features': 'sqrt', 'model__min_samples_leaf': 1, 'model__min_samples_split': 2}</t>
+  </si>
+  <si>
+    <t>0.792</t>
+  </si>
+  <si>
+    <t>0.893</t>
+  </si>
+  <si>
+    <t>20230228_1631_ExtraTrees_pca15</t>
+  </si>
+  <si>
+    <t>0.826</t>
+  </si>
+  <si>
+    <t>0.837</t>
+  </si>
+  <si>
+    <t>0.884</t>
+  </si>
+  <si>
+    <t>0.965</t>
+  </si>
+  <si>
+    <t>0.956</t>
+  </si>
+  <si>
+    <t>0.821</t>
+  </si>
+  <si>
+    <t>0.874</t>
+  </si>
+  <si>
+    <t>{'model__border_count': 64, 'model__depth': 8, 'model__iterations': 500, 'model__l2_leaf_reg': 1, 'model__learning_rate': 0.1}</t>
+  </si>
+  <si>
+    <t>0.894</t>
+  </si>
+  <si>
+    <t>{'model__border_count': 64, 'model__depth': 8, 'model__iterations': 500, 'model__l2_leaf_reg': 1, 'model__leaf_estimation_iterations': 10, 'model__learning_rate': 0.1, 'model__random_strength': 0.1}</t>
+  </si>
+  <si>
+    <t>scaling, euclidean_dist, linear_dist, mean_hillshade, morning_hillshade, mean_amenties, aspect_dir, climatic_zone, geologic_zone, soil_type</t>
+  </si>
+  <si>
+    <t>pca_components</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Corpo)"/>
+      </rPr>
+      <t xml:space="preserve">!!! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>In the submission  I did  said feat eng… the code was wrong, no feat eng, just pca on row data</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Corpo)"/>
+      </rPr>
+      <t xml:space="preserve">!!! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> In the submission  I did  said feat eng… the code was wrong, no feat eng, just pca on row data</t>
+    </r>
+  </si>
+  <si>
+    <t>Tuning Validation Acuuracy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="173" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -247,8 +398,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Corpo)"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,8 +431,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -270,21 +452,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -293,26 +508,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Valuta" xfId="1" builtinId="4"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="d/m/yy\ h:mm;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
@@ -337,21 +600,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}" name="Tabelle2" displayName="Tabelle2" ref="A1:K31" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:K31" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}" name="Tabelle2" displayName="Tabelle2" ref="A1:M55" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:M55" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{AE3501BC-A93F-A44E-91E9-C2C9630E4D3B}" name="Timestamp" dataDxfId="5">
       <calculatedColumnFormula>NOW()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{15C54594-C213-1040-BB39-08AD944E191F}" name="Modeling Type" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{648BE996-BCA1-8A48-875C-7BB80DC12EAC}" name="Submission Name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{15C54594-C213-1040-BB39-08AD944E191F}" name="Modeling Type" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{648BE996-BCA1-8A48-875C-7BB80DC12EAC}" name="Submission Name" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{5E4B52D5-07C9-6748-9EFB-13CFB56CC836}" name="Model"/>
     <tableColumn id="4" xr3:uid="{0CA337F9-6EAC-2245-A0E9-1CC0549A66D2}" name="data_enigneering"/>
     <tableColumn id="5" xr3:uid="{E165C24C-21E3-7746-ADCA-4046945B8FF4}" name="drop_original"/>
     <tableColumn id="6" xr3:uid="{5F373FDA-F78B-A445-AECD-2FBF1D911CBF}" name="hyperparameters"/>
-    <tableColumn id="7" xr3:uid="{57B2801D-A688-2F4B-BD21-80E36348E592}" name="(Mean CV) Train Accuracy" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{8A9A517A-9CA3-F94D-928C-325BD7B38657}" name="Mean CV Test Accuracy" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{62E583F3-DEF1-184A-B39C-7DD9F304B3F5}" name="Kaggle Score" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{1C5756B4-1E9A-914F-AFD3-36F356708C8A}" name="pca_components" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{57B2801D-A688-2F4B-BD21-80E36348E592}" name="(Mean CV) Train Accuracy" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{8A9A517A-9CA3-F94D-928C-325BD7B38657}" name="Mean CV Test Accuracy" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{15836FAE-9F60-B74F-A533-0DDFD4E8E3E5}" name="Tuning Validation Acuuracy" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{62E583F3-DEF1-184A-B39C-7DD9F304B3F5}" name="Kaggle Score" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{2C5DD473-C08D-2248-8F07-9BB79E2E24F3}" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -655,10 +920,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA64AB39-C08B-144A-A441-ED0863E84DF0}">
-  <dimension ref="A1:L32"/>
+  <sheetPr codeName="Foglio1"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="114" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,50 +935,58 @@
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="21">
         <v>44973.683333333334</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -733,24 +1007,26 @@
       <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="25"/>
+      <c r="I2" s="15">
         <v>0.7</v>
       </c>
-      <c r="I2" s="7">
+      <c r="J2" s="15">
         <v>0.7</v>
       </c>
-      <c r="J2" s="7">
+      <c r="K2" s="15"/>
+      <c r="L2" s="16">
         <v>0.71</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="22">
         <v>44971.897916666669</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -763,18 +1039,19 @@
       <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="8">
+      <c r="I3" s="5">
         <v>0.70899999999999996</v>
       </c>
-      <c r="I3" s="8">
+      <c r="J3" s="5">
         <v>0.70199999999999996</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="22">
         <v>44971.910416666666</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -787,18 +1064,19 @@
       <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="8">
+      <c r="I4" s="5">
         <v>0.98899999999999999</v>
       </c>
-      <c r="I4" s="8">
+      <c r="J4" s="5">
         <v>0.85699999999999998</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" s="17"/>
+      <c r="M4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="22">
         <v>44971.919444444444</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -814,18 +1092,19 @@
       <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="8">
+      <c r="I5" s="5">
         <v>0.996</v>
       </c>
-      <c r="I5" s="8">
+      <c r="J5" s="5">
         <v>0.85599999999999998</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" s="17"/>
+      <c r="M5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="22">
         <v>44971.920138888891</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -843,19 +1122,18 @@
       <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="5">
         <v>0.99099999999999999</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="6">
+      <c r="L6" s="17">
         <v>0.55600000000000005</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="22">
         <v>44971.930555555555</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -871,18 +1149,19 @@
       <c r="G7" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I7" s="5">
         <v>0.86499999999999999</v>
       </c>
-      <c r="I7" s="8">
+      <c r="J7" s="5">
         <v>0.80100000000000005</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" s="17"/>
+      <c r="M7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="22">
         <v>44971.931250000001</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -898,19 +1177,18 @@
       <c r="G8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="5">
         <v>0.86299999999999999</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8">
+      <c r="L8" s="17">
         <v>0.50765000000000005</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="22">
         <v>44971.939583333333</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -923,19 +1201,18 @@
       <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="8">
+      <c r="I9" s="5">
         <v>0.70799999999999996</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="6">
+      <c r="L9" s="17">
         <v>0.42299999999999999</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="22">
         <v>44971.973611111112</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -951,18 +1228,19 @@
       <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="8">
+      <c r="I10" s="5">
         <v>0.95599999999999996</v>
       </c>
-      <c r="I10" s="8">
+      <c r="J10" s="5">
         <v>0.86499999999999999</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" s="17"/>
+      <c r="M10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="22">
         <v>44971.974999999999</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -978,19 +1256,18 @@
       <c r="F11" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="8">
+      <c r="I11" s="5">
         <v>0.95</v>
       </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="6">
+      <c r="L11" s="17">
         <v>0.55500000000000005</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="22">
         <v>44977.675694444442</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1003,18 +1280,19 @@
       <c r="E12" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="I12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="L12" s="17"/>
+      <c r="M12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="22">
         <v>44977.677777777775</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1029,17 +1307,16 @@
       <c r="E13" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="6">
+      <c r="I13" s="5"/>
+      <c r="L13" s="17">
         <v>0.81423999999999996</v>
       </c>
-      <c r="K13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="M13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="22">
         <v>44979.9</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1052,18 +1329,19 @@
       <c r="E14" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="8">
+      <c r="I14" s="5">
         <v>1</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="J14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="L14" s="17"/>
+      <c r="M14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="22">
         <v>44979.900694444441</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1076,18 +1354,19 @@
       <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="8">
+      <c r="I15" s="5">
         <v>1</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="J15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="L15" s="17"/>
+      <c r="M15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="22">
         <v>44979.907638888886</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1102,18 +1381,18 @@
       <c r="E16" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="8">
+      <c r="I16" s="5">
         <v>1</v>
       </c>
-      <c r="J16" s="6">
+      <c r="L16" s="17">
         <v>0.64946999999999999</v>
       </c>
-      <c r="K16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="M16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="22">
         <v>44979.915972222225</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1129,24 +1408,24 @@
       <c r="G17" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="K17" t="s">
-        <v>12</v>
-      </c>
-      <c r="L17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="I17" s="5"/>
+      <c r="K17" s="5">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="L17" s="17"/>
+      <c r="M17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="22">
         <v>44979.930555555555</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
         <v>38</v>
@@ -1157,19 +1436,18 @@
       <c r="G18" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="8">
+      <c r="I18" s="5">
         <v>1</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="6">
+      <c r="L18" s="17">
         <v>0.82843999999999995</v>
       </c>
-      <c r="K18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="M18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="22">
         <v>44979.956944444442</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1183,26 +1461,26 @@
         <v>35</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="K19" t="s">
-        <v>12</v>
-      </c>
-      <c r="L19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+        <v>45</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="K19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="17"/>
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="22">
         <v>44979.959027777775</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
         <v>38</v>
@@ -1211,21 +1489,21 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="8">
+        <v>45</v>
+      </c>
+      <c r="I20" s="5">
         <v>1</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="6">
+      <c r="K20" s="4"/>
+      <c r="L20" s="17">
         <v>0.82972999999999997</v>
       </c>
-      <c r="K20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="M20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="22">
         <v>44979.969444444447</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1239,26 +1517,26 @@
         <v>35</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="K21" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="I21" s="5"/>
+      <c r="K21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L21" s="17"/>
+      <c r="M21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="22">
         <v>44980.959027777775</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
@@ -1267,21 +1545,21 @@
         <v>35</v>
       </c>
       <c r="G22" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="8">
+        <v>48</v>
+      </c>
+      <c r="I22" s="5">
         <v>1</v>
       </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="6">
+      <c r="K22" s="4"/>
+      <c r="L22" s="17">
         <v>0.83438000000000001</v>
       </c>
-      <c r="K22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="M22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="22">
         <v>44979.376388888886</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1295,26 +1573,26 @@
         <v>35</v>
       </c>
       <c r="G23" t="s">
-        <v>51</v>
-      </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="K23" t="s">
-        <v>12</v>
-      </c>
-      <c r="L23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+        <v>50</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="K23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L23" s="17"/>
+      <c r="M23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="22">
         <v>44979.416666666664</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
@@ -1323,21 +1601,21 @@
         <v>35</v>
       </c>
       <c r="G24" t="s">
-        <v>51</v>
-      </c>
-      <c r="H24" s="8">
+        <v>50</v>
+      </c>
+      <c r="I24" s="5">
         <v>1</v>
       </c>
-      <c r="I24" s="8"/>
-      <c r="J24" s="6">
+      <c r="K24" s="4"/>
+      <c r="L24" s="17">
         <v>0.83453999999999995</v>
       </c>
-      <c r="K24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="M24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="22">
         <v>44981.481944444444</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1350,18 +1628,20 @@
       <c r="E25" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="8">
+      <c r="I25" s="5">
         <v>0.85799999999999998</v>
       </c>
-      <c r="I25" s="6">
+      <c r="J25" s="5">
         <v>0.78400000000000003</v>
       </c>
-      <c r="K25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="K25" s="4"/>
+      <c r="L25" s="17"/>
+      <c r="M25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="22">
         <v>44981.506944444445</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1375,49 +1655,49 @@
         <v>35</v>
       </c>
       <c r="G26" t="s">
-        <v>54</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="K26" t="s">
-        <v>12</v>
-      </c>
-      <c r="L26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+        <v>53</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="K26" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L26" s="17"/>
+      <c r="M26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="22">
         <v>44981.513194444444</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E27" t="s">
         <v>35</v>
       </c>
       <c r="G27" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="8">
+        <v>53</v>
+      </c>
+      <c r="I27" s="5">
         <v>1</v>
       </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="10">
+      <c r="K27" s="4"/>
+      <c r="L27" s="29">
         <v>0.83076000000000005</v>
       </c>
-      <c r="K27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="M27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="22">
         <v>44981.51666666667</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1431,67 +1711,786 @@
         <v>35</v>
       </c>
       <c r="G28" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="K28" t="s">
-        <v>12</v>
-      </c>
-      <c r="L28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+        <v>55</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="K28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L28" s="17"/>
+      <c r="M28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="22">
         <v>44981.57916666667</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E29" t="s">
         <v>35</v>
       </c>
       <c r="G29" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" s="8">
+        <v>55</v>
+      </c>
+      <c r="I29" s="5">
         <v>1</v>
       </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="10">
+      <c r="L29" s="18">
         <v>0.83511999999999997</v>
       </c>
-      <c r="K29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
+      <c r="M29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="22">
+        <v>44985.458333333336</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C30" s="1"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H31"/>
-      <c r="I31"/>
-      <c r="J31"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H32"/>
-      <c r="I32"/>
-      <c r="J32"/>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" s="26">
+        <v>15</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L30" s="17"/>
+      <c r="M30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="22">
+        <v>44985.477777777778</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="26">
+        <v>15</v>
+      </c>
+      <c r="I31" s="5">
+        <v>1</v>
+      </c>
+      <c r="L31" s="17">
+        <v>0.81272</v>
+      </c>
+      <c r="M31" t="s">
+        <v>12</v>
+      </c>
+      <c r="N31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="22">
+        <v>44985.513888888891</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="5">
+        <v>1</v>
+      </c>
+      <c r="J32" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="L32" s="17"/>
+      <c r="M32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="22">
+        <v>44985.517361111109</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="5">
+        <v>1</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="L33" s="17"/>
+      <c r="M33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="22">
+        <v>44985.519444444442</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" s="5">
+        <v>1</v>
+      </c>
+      <c r="J34" s="5">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="L34" s="17"/>
+      <c r="M34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="22">
+        <v>44985.520833333336</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" t="s">
+        <v>55</v>
+      </c>
+      <c r="I35" s="5">
+        <v>1</v>
+      </c>
+      <c r="J35" s="5">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="L35" s="17"/>
+      <c r="M35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="22">
+        <v>44985.52847222222</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36" s="5">
+        <v>1</v>
+      </c>
+      <c r="L36" s="17">
+        <v>0.82679000000000002</v>
+      </c>
+      <c r="M36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="22">
+        <v>44985.539583333331</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" t="s">
+        <v>64</v>
+      </c>
+      <c r="G37" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="5"/>
+      <c r="K37" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L37" s="17"/>
+      <c r="M37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="22">
+        <v>44985.622916666667</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K38" s="4"/>
+      <c r="L38" s="17"/>
+      <c r="M38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="22">
+        <v>44985.656944444447</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39" t="s">
+        <v>72</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="K39" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L39" s="17"/>
+      <c r="M39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="22">
+        <v>44985.659722222219</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40" t="s">
+        <v>72</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K40" s="4"/>
+      <c r="L40" s="17"/>
+      <c r="M40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="23">
+        <v>44985.665277777778</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L41" s="19"/>
+      <c r="M41" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="23">
+        <v>44985.666666666664</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" s="27"/>
+      <c r="I42" s="13">
+        <v>1</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K42" s="4"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="22">
+        <v>44985.677083333336</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H43" s="27"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L43" s="19"/>
+      <c r="M43" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="22">
+        <v>44985.677083333336</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H44" s="27"/>
+      <c r="I44" s="13">
+        <v>1</v>
+      </c>
+      <c r="J44" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K44" s="13"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="22">
+        <v>44985.677083333336</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H45" s="27">
+        <v>15</v>
+      </c>
+      <c r="I45" s="13">
+        <v>1</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K45" s="13"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="22">
+        <v>44985.688194444447</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H46" s="27">
+        <v>15</v>
+      </c>
+      <c r="I46" s="13">
+        <v>1</v>
+      </c>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="19">
+        <v>0.82506999999999997</v>
+      </c>
+      <c r="M46" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="22">
+        <v>44986.398611111108</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+      <c r="G47" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" s="26">
+        <v>15</v>
+      </c>
+      <c r="I47" s="5">
+        <v>1</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L47" s="17"/>
+      <c r="M47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="22">
+        <v>44986.398611111108</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H48" s="28">
+        <v>15</v>
+      </c>
+      <c r="I48" s="5">
+        <v>1</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L48" s="17"/>
+      <c r="M48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="22">
+        <v>44986.404861111114</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L49" s="17"/>
+      <c r="M49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="22">
+        <v>44986.406944444447</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H50" s="26">
+        <v>15</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L50" s="17"/>
+      <c r="M50" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="22">
+        <v>44986.411805555559</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51" t="s">
+        <v>90</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="K51" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="L51" s="17"/>
+      <c r="M51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="22">
+        <v>44986.430555555555</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" t="s">
+        <v>92</v>
+      </c>
+      <c r="I52" s="5"/>
+      <c r="K52" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L52" s="17"/>
+      <c r="M52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="22">
+        <v>44986.440972222219</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53" t="s">
+        <v>92</v>
+      </c>
+      <c r="I53" s="5">
+        <v>1</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="L53" s="17"/>
+      <c r="M53" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="22">
+        <v>44986.440972222219</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" t="s">
+        <v>93</v>
+      </c>
+      <c r="G54" t="s">
+        <v>55</v>
+      </c>
+      <c r="I54" s="5">
+        <v>1</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="L54" s="17"/>
+      <c r="M54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="22"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="I55" s="5"/>
+      <c r="L55" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1502,19 +2501,19 @@
           <x14:formula1>
             <xm:f>Dropdowns!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B30</xm:sqref>
+          <xm:sqref>B38:B46 B2:B36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5314795F-EFA8-DC48-AEC4-309F78D8EA79}">
           <x14:formula1>
             <xm:f>Dropdowns!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K30</xm:sqref>
+          <xm:sqref>M38 M40 M42 M2:M36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E773B72D-11B4-4543-9E3B-6D3AAA4F3477}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{82231E75-7DFD-C64F-B418-BB6F687712B9}">
           <x14:formula1>
-            <xm:f>Dropdowns!#REF!</xm:f>
+            <xm:f>Dropdowns!$E:$E</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D30</xm:sqref>
+          <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1524,10 +2523,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A561FA97-048C-B04D-9B19-9201C434118E}">
-  <dimension ref="A1:E9"/>
+  <sheetPr codeName="Foglio2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1593,12 +2593,17 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added first LCE test run
</commit_message>
<xml_diff>
--- a/modeling/modeling_tracker.xlsx
+++ b/modeling/modeling_tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianna/Documents/master/2022-2023/Machine_learning_2/ml2challenge/modeling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/Machine Learning II/ml2challenge/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8CE6B6-9AB6-FC49-A186-A85462F76E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186AA8E7-6A31-E347-AF03-2B5464C8DD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="99">
   <si>
     <t>hyperparameters</t>
   </si>
@@ -366,16 +366,19 @@
   <si>
     <t>Tuning Validation Acuuracy</t>
   </si>
+  <si>
+    <t>LCE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="173" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -492,9 +495,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -502,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -514,74 +517,69 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Valuta" xfId="1" builtinId="4"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <numFmt numFmtId="166" formatCode="0.00000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.00000"/>
+      <numFmt numFmtId="165" formatCode="0.000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode="d/m/yy\ h:mm;@"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+      <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -603,20 +601,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}" name="Tabelle2" displayName="Tabelle2" ref="A1:M55" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:M55" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AE3501BC-A93F-A44E-91E9-C2C9630E4D3B}" name="Timestamp" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{AE3501BC-A93F-A44E-91E9-C2C9630E4D3B}" name="Timestamp" dataDxfId="7">
       <calculatedColumnFormula>NOW()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{15C54594-C213-1040-BB39-08AD944E191F}" name="Modeling Type" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{648BE996-BCA1-8A48-875C-7BB80DC12EAC}" name="Submission Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{15C54594-C213-1040-BB39-08AD944E191F}" name="Modeling Type" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{648BE996-BCA1-8A48-875C-7BB80DC12EAC}" name="Submission Name" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{5E4B52D5-07C9-6748-9EFB-13CFB56CC836}" name="Model"/>
     <tableColumn id="4" xr3:uid="{0CA337F9-6EAC-2245-A0E9-1CC0549A66D2}" name="data_enigneering"/>
     <tableColumn id="5" xr3:uid="{E165C24C-21E3-7746-ADCA-4046945B8FF4}" name="drop_original"/>
     <tableColumn id="6" xr3:uid="{5F373FDA-F78B-A445-AECD-2FBF1D911CBF}" name="hyperparameters"/>
-    <tableColumn id="12" xr3:uid="{1C5756B4-1E9A-914F-AFD3-36F356708C8A}" name="pca_components" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{57B2801D-A688-2F4B-BD21-80E36348E592}" name="(Mean CV) Train Accuracy" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{1C5756B4-1E9A-914F-AFD3-36F356708C8A}" name="pca_components" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{57B2801D-A688-2F4B-BD21-80E36348E592}" name="(Mean CV) Train Accuracy" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{8A9A517A-9CA3-F94D-928C-325BD7B38657}" name="Mean CV Test Accuracy" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{15836FAE-9F60-B74F-A533-0DDFD4E8E3E5}" name="Tuning Validation Acuuracy" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{62E583F3-DEF1-184A-B39C-7DD9F304B3F5}" name="Kaggle Score" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{15836FAE-9F60-B74F-A533-0DDFD4E8E3E5}" name="Tuning Validation Acuuracy" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{62E583F3-DEF1-184A-B39C-7DD9F304B3F5}" name="Kaggle Score" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{2C5DD473-C08D-2248-8F07-9BB79E2E24F3}" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -624,7 +622,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -923,8 +921,8 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="114" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="88" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -936,7 +934,7 @@
     <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.5" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.83203125" style="5" customWidth="1"/>
@@ -966,13 +964,13 @@
       <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>94</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="19" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -986,7 +984,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="21">
+      <c r="A2" s="20">
         <v>44973.683333333334</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1007,15 +1005,15 @@
       <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="15">
+      <c r="H2" s="24"/>
+      <c r="I2" s="14">
         <v>0.7</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="14">
         <v>0.7</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="16">
+      <c r="K2" s="14"/>
+      <c r="L2" s="15">
         <v>0.71</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1026,7 +1024,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="22">
+      <c r="A3" s="21">
         <v>44971.897916666669</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1045,13 +1043,13 @@
       <c r="J3" s="5">
         <v>0.70199999999999996</v>
       </c>
-      <c r="L3" s="17"/>
+      <c r="L3" s="16"/>
       <c r="M3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>44971.910416666666</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1070,13 +1068,13 @@
       <c r="J4" s="5">
         <v>0.85699999999999998</v>
       </c>
-      <c r="L4" s="17"/>
+      <c r="L4" s="16"/>
       <c r="M4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>44971.919444444444</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1098,13 +1096,13 @@
       <c r="J5" s="5">
         <v>0.85599999999999998</v>
       </c>
-      <c r="L5" s="17"/>
+      <c r="L5" s="16"/>
       <c r="M5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>44971.920138888891</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1125,7 +1123,7 @@
       <c r="I6" s="5">
         <v>0.99099999999999999</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="16">
         <v>0.55600000000000005</v>
       </c>
       <c r="M6" t="s">
@@ -1133,7 +1131,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>44971.930555555555</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1155,13 +1153,13 @@
       <c r="J7" s="5">
         <v>0.80100000000000005</v>
       </c>
-      <c r="L7" s="17"/>
+      <c r="L7" s="16"/>
       <c r="M7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="22">
+      <c r="A8" s="21">
         <v>44971.931250000001</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1180,7 +1178,7 @@
       <c r="I8" s="5">
         <v>0.86299999999999999</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <v>0.50765000000000005</v>
       </c>
       <c r="M8" t="s">
@@ -1188,7 +1186,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="22">
+      <c r="A9" s="21">
         <v>44971.939583333333</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1204,7 +1202,7 @@
       <c r="I9" s="5">
         <v>0.70799999999999996</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="16">
         <v>0.42299999999999999</v>
       </c>
       <c r="M9" t="s">
@@ -1212,7 +1210,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="22">
+      <c r="A10" s="21">
         <v>44971.973611111112</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1234,13 +1232,13 @@
       <c r="J10" s="5">
         <v>0.86499999999999999</v>
       </c>
-      <c r="L10" s="17"/>
+      <c r="L10" s="16"/>
       <c r="M10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="22">
+      <c r="A11" s="21">
         <v>44971.974999999999</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1259,7 +1257,7 @@
       <c r="I11" s="5">
         <v>0.95</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="16">
         <v>0.55500000000000005</v>
       </c>
       <c r="M11" t="s">
@@ -1267,7 +1265,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="22">
+      <c r="A12" s="21">
         <v>44977.675694444442</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1286,13 +1284,13 @@
       <c r="J12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="17"/>
+      <c r="L12" s="16"/>
       <c r="M12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="22">
+      <c r="A13" s="21">
         <v>44977.677777777775</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1308,7 +1306,7 @@
         <v>35</v>
       </c>
       <c r="I13" s="5"/>
-      <c r="L13" s="17">
+      <c r="L13" s="16">
         <v>0.81423999999999996</v>
       </c>
       <c r="M13" t="s">
@@ -1316,7 +1314,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="22">
+      <c r="A14" s="21">
         <v>44979.9</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1335,13 +1333,13 @@
       <c r="J14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L14" s="17"/>
+      <c r="L14" s="16"/>
       <c r="M14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="22">
+      <c r="A15" s="21">
         <v>44979.900694444441</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1360,13 +1358,13 @@
       <c r="J15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="17"/>
+      <c r="L15" s="16"/>
       <c r="M15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="22">
+      <c r="A16" s="21">
         <v>44979.907638888886</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1384,7 +1382,7 @@
       <c r="I16" s="5">
         <v>1</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="16">
         <v>0.64946999999999999</v>
       </c>
       <c r="M16" t="s">
@@ -1392,7 +1390,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="22">
+      <c r="A17" s="21">
         <v>44979.915972222225</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1412,13 +1410,13 @@
       <c r="K17" s="5">
         <v>0.90300000000000002</v>
       </c>
-      <c r="L17" s="17"/>
+      <c r="L17" s="16"/>
       <c r="M17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="22">
+      <c r="A18" s="21">
         <v>44979.930555555555</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1439,7 +1437,7 @@
       <c r="I18" s="5">
         <v>1</v>
       </c>
-      <c r="L18" s="17">
+      <c r="L18" s="16">
         <v>0.82843999999999995</v>
       </c>
       <c r="M18" t="s">
@@ -1447,7 +1445,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="22">
+      <c r="A19" s="21">
         <v>44979.956944444442</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1467,13 +1465,13 @@
       <c r="K19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L19" s="17"/>
+      <c r="L19" s="16"/>
       <c r="M19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="22">
+      <c r="A20" s="21">
         <v>44979.959027777775</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1495,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="4"/>
-      <c r="L20" s="17">
+      <c r="L20" s="16">
         <v>0.82972999999999997</v>
       </c>
       <c r="M20" t="s">
@@ -1503,7 +1501,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="22">
+      <c r="A21" s="21">
         <v>44979.969444444447</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1523,13 +1521,13 @@
       <c r="K21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L21" s="17"/>
+      <c r="L21" s="16"/>
       <c r="M21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="22">
+      <c r="A22" s="21">
         <v>44980.959027777775</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1551,7 +1549,7 @@
         <v>1</v>
       </c>
       <c r="K22" s="4"/>
-      <c r="L22" s="17">
+      <c r="L22" s="16">
         <v>0.83438000000000001</v>
       </c>
       <c r="M22" t="s">
@@ -1559,7 +1557,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="22">
+      <c r="A23" s="21">
         <v>44979.376388888886</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1579,13 +1577,13 @@
       <c r="K23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L23" s="17"/>
+      <c r="L23" s="16"/>
       <c r="M23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="22">
+      <c r="A24" s="21">
         <v>44979.416666666664</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1607,7 +1605,7 @@
         <v>1</v>
       </c>
       <c r="K24" s="4"/>
-      <c r="L24" s="17">
+      <c r="L24" s="16">
         <v>0.83453999999999995</v>
       </c>
       <c r="M24" t="s">
@@ -1615,7 +1613,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="22">
+      <c r="A25" s="21">
         <v>44981.481944444444</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1635,13 +1633,13 @@
         <v>0.78400000000000003</v>
       </c>
       <c r="K25" s="4"/>
-      <c r="L25" s="17"/>
+      <c r="L25" s="16"/>
       <c r="M25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="22">
+      <c r="A26" s="21">
         <v>44981.506944444445</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1661,13 +1659,13 @@
       <c r="K26" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L26" s="17"/>
+      <c r="L26" s="16"/>
       <c r="M26" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="22">
+      <c r="A27" s="21">
         <v>44981.513194444444</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1676,7 +1674,7 @@
       <c r="C27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" t="s">
         <v>38</v>
       </c>
       <c r="E27" t="s">
@@ -1689,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="4"/>
-      <c r="L27" s="29">
+      <c r="L27" s="16">
         <v>0.83076000000000005</v>
       </c>
       <c r="M27" t="s">
@@ -1697,7 +1695,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="22">
+      <c r="A28" s="21">
         <v>44981.51666666667</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1717,13 +1715,13 @@
       <c r="K28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L28" s="17"/>
+      <c r="L28" s="16"/>
       <c r="M28" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="22">
+      <c r="A29" s="21">
         <v>44981.57916666667</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1744,7 +1742,7 @@
       <c r="I29" s="5">
         <v>1</v>
       </c>
-      <c r="L29" s="18">
+      <c r="L29" s="17">
         <v>0.83511999999999997</v>
       </c>
       <c r="M29" t="s">
@@ -1752,7 +1750,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="22">
+      <c r="A30" s="21">
         <v>44985.458333333336</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1765,7 +1763,7 @@
       <c r="G30" t="s">
         <v>55</v>
       </c>
-      <c r="H30" s="26">
+      <c r="H30" s="25">
         <v>15</v>
       </c>
       <c r="I30" s="5">
@@ -1774,13 +1772,13 @@
       <c r="J30" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L30" s="17"/>
+      <c r="L30" s="16"/>
       <c r="M30" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="22">
+      <c r="A31" s="21">
         <v>44985.477777777778</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1795,13 +1793,13 @@
       <c r="G31" t="s">
         <v>55</v>
       </c>
-      <c r="H31" s="26">
+      <c r="H31" s="25">
         <v>15</v>
       </c>
       <c r="I31" s="5">
         <v>1</v>
       </c>
-      <c r="L31" s="17">
+      <c r="L31" s="16">
         <v>0.81272</v>
       </c>
       <c r="M31" t="s">
@@ -1812,7 +1810,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="22">
+      <c r="A32" s="21">
         <v>44985.513888888891</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1834,13 +1832,13 @@
       <c r="J32" s="5">
         <v>0.9</v>
       </c>
-      <c r="L32" s="17"/>
+      <c r="L32" s="16"/>
       <c r="M32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="22">
+      <c r="A33" s="21">
         <v>44985.517361111109</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1862,13 +1860,13 @@
       <c r="J33" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L33" s="17"/>
+      <c r="L33" s="16"/>
       <c r="M33" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="22">
+      <c r="A34" s="21">
         <v>44985.519444444442</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1893,13 +1891,13 @@
       <c r="J34" s="5">
         <v>0.90100000000000002</v>
       </c>
-      <c r="L34" s="17"/>
+      <c r="L34" s="16"/>
       <c r="M34" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="22">
+      <c r="A35" s="21">
         <v>44985.520833333336</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1924,13 +1922,13 @@
       <c r="J35" s="5">
         <v>0.89700000000000002</v>
       </c>
-      <c r="L35" s="17"/>
+      <c r="L35" s="16"/>
       <c r="M35" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="22">
+      <c r="A36" s="21">
         <v>44985.52847222222</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1954,7 +1952,7 @@
       <c r="I36" s="5">
         <v>1</v>
       </c>
-      <c r="L36" s="17">
+      <c r="L36" s="16">
         <v>0.82679000000000002</v>
       </c>
       <c r="M36" t="s">
@@ -1962,7 +1960,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37" s="22">
+      <c r="A37" s="21">
         <v>44985.539583333331</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1985,13 +1983,13 @@
       <c r="K37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L37" s="17"/>
+      <c r="L37" s="16"/>
       <c r="M37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="22">
+      <c r="A38" s="21">
         <v>44985.622916666667</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2011,13 +2009,13 @@
         <v>70</v>
       </c>
       <c r="K38" s="4"/>
-      <c r="L38" s="17"/>
+      <c r="L38" s="16"/>
       <c r="M38" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="22">
+      <c r="A39" s="21">
         <v>44985.656944444447</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2037,13 +2035,13 @@
       <c r="K39" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="L39" s="17"/>
+      <c r="L39" s="16"/>
       <c r="M39" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="22">
+      <c r="A40" s="21">
         <v>44985.659722222219</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2066,13 +2064,13 @@
         <v>74</v>
       </c>
       <c r="K40" s="4"/>
-      <c r="L40" s="17"/>
+      <c r="L40" s="16"/>
       <c r="M40" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="23">
+      <c r="A41" s="22">
         <v>44985.665277777778</v>
       </c>
       <c r="B41" s="12" t="s">
@@ -2087,19 +2085,19 @@
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="27"/>
+      <c r="H41" s="26"/>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
       <c r="K41" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="L41" s="19"/>
+      <c r="L41" s="18"/>
       <c r="M41" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="23">
+      <c r="A42" s="22">
         <v>44985.666666666664</v>
       </c>
       <c r="B42" s="12" t="s">
@@ -2116,7 +2114,7 @@
       <c r="G42" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H42" s="27"/>
+      <c r="H42" s="26"/>
       <c r="I42" s="13">
         <v>1</v>
       </c>
@@ -2124,13 +2122,13 @@
         <v>77</v>
       </c>
       <c r="K42" s="4"/>
-      <c r="L42" s="19"/>
+      <c r="L42" s="18"/>
       <c r="M42" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="22">
+      <c r="A43" s="21">
         <v>44985.677083333336</v>
       </c>
       <c r="B43" s="12" t="s">
@@ -2147,19 +2145,19 @@
       <c r="G43" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H43" s="27"/>
+      <c r="H43" s="26"/>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
       <c r="K43" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="L43" s="19"/>
+      <c r="L43" s="18"/>
       <c r="M43" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="22">
+      <c r="A44" s="21">
         <v>44985.677083333336</v>
       </c>
       <c r="B44" s="12" t="s">
@@ -2176,7 +2174,7 @@
       <c r="G44" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H44" s="27"/>
+      <c r="H44" s="26"/>
       <c r="I44" s="13">
         <v>1</v>
       </c>
@@ -2184,13 +2182,13 @@
         <v>80</v>
       </c>
       <c r="K44" s="13"/>
-      <c r="L44" s="19"/>
+      <c r="L44" s="18"/>
       <c r="M44" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="22">
+      <c r="A45" s="21">
         <v>44985.677083333336</v>
       </c>
       <c r="B45" s="12" t="s">
@@ -2205,7 +2203,7 @@
       <c r="G45" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H45" s="27">
+      <c r="H45" s="26">
         <v>15</v>
       </c>
       <c r="I45" s="13">
@@ -2215,13 +2213,13 @@
         <v>81</v>
       </c>
       <c r="K45" s="13"/>
-      <c r="L45" s="19"/>
+      <c r="L45" s="18"/>
       <c r="M45" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="22">
+      <c r="A46" s="21">
         <v>44985.688194444447</v>
       </c>
       <c r="B46" s="12" t="s">
@@ -2238,7 +2236,7 @@
       <c r="G46" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H46" s="27">
+      <c r="H46" s="26">
         <v>15</v>
       </c>
       <c r="I46" s="13">
@@ -2246,7 +2244,7 @@
       </c>
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>
-      <c r="L46" s="19">
+      <c r="L46" s="18">
         <v>0.82506999999999997</v>
       </c>
       <c r="M46" s="9" t="s">
@@ -2257,7 +2255,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="22">
+      <c r="A47" s="21">
         <v>44986.398611111108</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2273,7 +2271,7 @@
       <c r="G47" t="s">
         <v>55</v>
       </c>
-      <c r="H47" s="26">
+      <c r="H47" s="25">
         <v>15</v>
       </c>
       <c r="I47" s="5">
@@ -2282,30 +2280,29 @@
       <c r="J47" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="L47" s="17"/>
+      <c r="L47" s="16"/>
       <c r="M47" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="22">
+      <c r="A48" s="21">
         <v>44986.398611111108</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="14" t="s">
+      <c r="D48" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14" t="s">
+      <c r="G48" t="s">
         <v>53</v>
       </c>
-      <c r="H48" s="28">
+      <c r="H48" s="25">
         <v>15</v>
       </c>
       <c r="I48" s="5">
@@ -2314,13 +2311,13 @@
       <c r="J48" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="L48" s="17"/>
+      <c r="L48" s="16"/>
       <c r="M48" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="22">
+      <c r="A49" s="21">
         <v>44986.404861111114</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2330,7 +2327,7 @@
       <c r="D49" t="s">
         <v>16</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="E49" t="s">
         <v>35</v>
       </c>
       <c r="I49" s="5" t="s">
@@ -2339,13 +2336,13 @@
       <c r="J49" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="L49" s="17"/>
+      <c r="L49" s="16"/>
       <c r="M49" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="22">
+      <c r="A50" s="21">
         <v>44986.406944444447</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2355,10 +2352,10 @@
       <c r="D50" t="s">
         <v>16</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" t="s">
         <v>35</v>
       </c>
-      <c r="H50" s="26">
+      <c r="H50" s="25">
         <v>15</v>
       </c>
       <c r="I50" s="5" t="s">
@@ -2367,13 +2364,13 @@
       <c r="J50" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="L50" s="17"/>
+      <c r="L50" s="16"/>
       <c r="M50" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="22">
+      <c r="A51" s="21">
         <v>44986.411805555559</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2383,7 +2380,7 @@
       <c r="D51" t="s">
         <v>16</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" t="s">
         <v>35</v>
       </c>
       <c r="G51" t="s">
@@ -2393,13 +2390,13 @@
       <c r="K51" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L51" s="17"/>
+      <c r="L51" s="16"/>
       <c r="M51" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="22">
+      <c r="A52" s="21">
         <v>44986.430555555555</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2409,7 +2406,7 @@
       <c r="D52" t="s">
         <v>16</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="E52" t="s">
         <v>35</v>
       </c>
       <c r="G52" t="s">
@@ -2419,13 +2416,13 @@
       <c r="K52" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="L52" s="17"/>
+      <c r="L52" s="16"/>
       <c r="M52" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="22">
+      <c r="A53" s="21">
         <v>44986.440972222219</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2435,7 +2432,7 @@
       <c r="D53" t="s">
         <v>16</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" t="s">
         <v>35</v>
       </c>
       <c r="G53" t="s">
@@ -2447,13 +2444,13 @@
       <c r="J53" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="L53" s="17"/>
+      <c r="L53" s="16"/>
       <c r="M53" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="22">
+      <c r="A54" s="21">
         <v>44986.440972222219</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2475,17 +2472,35 @@
       <c r="J54" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="L54" s="17"/>
+      <c r="L54" s="16"/>
       <c r="M54" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="22"/>
-      <c r="B55" s="1"/>
+      <c r="A55" s="21">
+        <v>44988.951388888891</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C55" s="1"/>
-      <c r="I55" s="5"/>
-      <c r="L55" s="17"/>
+      <c r="D55" t="s">
+        <v>98</v>
+      </c>
+      <c r="E55" t="s">
+        <v>33</v>
+      </c>
+      <c r="I55" s="5">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="J55" s="5">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="L55" s="16"/>
+      <c r="M55" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2513,7 +2528,7 @@
           <x14:formula1>
             <xm:f>Dropdowns!$E:$E</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D1048576</xm:sqref>
+          <xm:sqref>D1 D56:D1048576 D2:D55</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2524,10 +2539,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A561FA97-048C-B04D-9B19-9201C434118E}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2606,6 +2621,11 @@
         <v>75</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tests and submission for mean agg over train data
</commit_message>
<xml_diff>
--- a/modeling/modeling_tracker.xlsx
+++ b/modeling/modeling_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/Machine Learning II/ml2challenge/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186AA8E7-6A31-E347-AF03-2B5464C8DD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F34A8F-46AA-6346-8EF7-50FA6F73D227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="103">
   <si>
     <t>hyperparameters</t>
   </si>
@@ -368,6 +368,18 @@
   </si>
   <si>
     <t>LCE</t>
+  </si>
+  <si>
+    <t>euclidean_dist, linear_dist, mean_hillshade, morning_hillshade, mean_amenties, aspect_dir, climatic_zone, geologic_zone, soil_type, aggregate_elevation</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>predefined mean for Elevation per wilderniss area</t>
+  </si>
+  <si>
+    <t>predefined mean for Elevation per soiltype</t>
   </si>
 </sst>
 </file>
@@ -552,7 +564,11 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.00000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -598,24 +614,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}" name="Tabelle2" displayName="Tabelle2" ref="A1:M55" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:M55" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AE3501BC-A93F-A44E-91E9-C2C9630E4D3B}" name="Timestamp" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}" name="Tabelle2" displayName="Tabelle2" ref="A1:N59" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:N59" xr:uid="{90303A0C-EE9B-7B43-94DD-90FEB1417FBF}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{AE3501BC-A93F-A44E-91E9-C2C9630E4D3B}" name="Timestamp" dataDxfId="8">
       <calculatedColumnFormula>NOW()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{15C54594-C213-1040-BB39-08AD944E191F}" name="Modeling Type" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{648BE996-BCA1-8A48-875C-7BB80DC12EAC}" name="Submission Name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{15C54594-C213-1040-BB39-08AD944E191F}" name="Modeling Type" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{648BE996-BCA1-8A48-875C-7BB80DC12EAC}" name="Submission Name" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{5E4B52D5-07C9-6748-9EFB-13CFB56CC836}" name="Model"/>
     <tableColumn id="4" xr3:uid="{0CA337F9-6EAC-2245-A0E9-1CC0549A66D2}" name="data_enigneering"/>
     <tableColumn id="5" xr3:uid="{E165C24C-21E3-7746-ADCA-4046945B8FF4}" name="drop_original"/>
     <tableColumn id="6" xr3:uid="{5F373FDA-F78B-A445-AECD-2FBF1D911CBF}" name="hyperparameters"/>
-    <tableColumn id="12" xr3:uid="{1C5756B4-1E9A-914F-AFD3-36F356708C8A}" name="pca_components" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{57B2801D-A688-2F4B-BD21-80E36348E592}" name="(Mean CV) Train Accuracy" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{8A9A517A-9CA3-F94D-928C-325BD7B38657}" name="Mean CV Test Accuracy" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{15836FAE-9F60-B74F-A533-0DDFD4E8E3E5}" name="Tuning Validation Acuuracy" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{62E583F3-DEF1-184A-B39C-7DD9F304B3F5}" name="Kaggle Score" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{2C5DD473-C08D-2248-8F07-9BB79E2E24F3}" name="Author"/>
+    <tableColumn id="12" xr3:uid="{1C5756B4-1E9A-914F-AFD3-36F356708C8A}" name="pca_components" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{57B2801D-A688-2F4B-BD21-80E36348E592}" name="(Mean CV) Train Accuracy" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{8A9A517A-9CA3-F94D-928C-325BD7B38657}" name="Mean CV Test Accuracy" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{15836FAE-9F60-B74F-A533-0DDFD4E8E3E5}" name="Tuning Validation Acuuracy" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{62E583F3-DEF1-184A-B39C-7DD9F304B3F5}" name="Kaggle Score" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{51D38C06-A2C6-624C-B351-4398128C6F8E}" name="Author" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{2C5DD473-C08D-2248-8F07-9BB79E2E24F3}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -919,10 +936,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA64AB39-C08B-144A-A441-ED0863E84DF0}">
   <sheetPr codeName="Foglio1"/>
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="88" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="88" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -939,10 +956,11 @@
     <col min="10" max="10" width="23.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.83203125" style="5" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="85.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -982,8 +1000,11 @@
       <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N1" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="20">
         <v>44973.683333333334</v>
       </c>
@@ -1016,14 +1037,15 @@
       <c r="L2" s="15">
         <v>0.71</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="15" t="s">
         <v>14</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="21">
         <v>44971.897916666669</v>
       </c>
@@ -1044,11 +1066,11 @@
         <v>0.70199999999999996</v>
       </c>
       <c r="L3" s="16"/>
-      <c r="M3" t="s">
+      <c r="M3" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="21">
         <v>44971.910416666666</v>
       </c>
@@ -1069,11 +1091,11 @@
         <v>0.85699999999999998</v>
       </c>
       <c r="L4" s="16"/>
-      <c r="M4" t="s">
+      <c r="M4" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="21">
         <v>44971.919444444444</v>
       </c>
@@ -1097,11 +1119,11 @@
         <v>0.85599999999999998</v>
       </c>
       <c r="L5" s="16"/>
-      <c r="M5" t="s">
+      <c r="M5" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="21">
         <v>44971.920138888891</v>
       </c>
@@ -1126,11 +1148,11 @@
       <c r="L6" s="16">
         <v>0.55600000000000005</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="21">
         <v>44971.930555555555</v>
       </c>
@@ -1154,11 +1176,11 @@
         <v>0.80100000000000005</v>
       </c>
       <c r="L7" s="16"/>
-      <c r="M7" t="s">
+      <c r="M7" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="21">
         <v>44971.931250000001</v>
       </c>
@@ -1181,11 +1203,11 @@
       <c r="L8" s="16">
         <v>0.50765000000000005</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="21">
         <v>44971.939583333333</v>
       </c>
@@ -1205,11 +1227,11 @@
       <c r="L9" s="16">
         <v>0.42299999999999999</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="21">
         <v>44971.973611111112</v>
       </c>
@@ -1233,11 +1255,11 @@
         <v>0.86499999999999999</v>
       </c>
       <c r="L10" s="16"/>
-      <c r="M10" t="s">
+      <c r="M10" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="21">
         <v>44971.974999999999</v>
       </c>
@@ -1260,11 +1282,11 @@
       <c r="L11" s="16">
         <v>0.55500000000000005</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="21">
         <v>44977.675694444442</v>
       </c>
@@ -1285,11 +1307,11 @@
         <v>36</v>
       </c>
       <c r="L12" s="16"/>
-      <c r="M12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M12" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="21">
         <v>44977.677777777775</v>
       </c>
@@ -1309,11 +1331,11 @@
       <c r="L13" s="16">
         <v>0.81423999999999996</v>
       </c>
-      <c r="M13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M13" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="21">
         <v>44979.9</v>
       </c>
@@ -1334,11 +1356,11 @@
         <v>39</v>
       </c>
       <c r="L14" s="16"/>
-      <c r="M14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M14" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="21">
         <v>44979.900694444441</v>
       </c>
@@ -1359,11 +1381,11 @@
         <v>40</v>
       </c>
       <c r="L15" s="16"/>
-      <c r="M15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M15" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="21">
         <v>44979.907638888886</v>
       </c>
@@ -1385,7 +1407,7 @@
       <c r="L16" s="16">
         <v>0.64946999999999999</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1411,7 +1433,7 @@
         <v>0.90300000000000002</v>
       </c>
       <c r="L17" s="16"/>
-      <c r="M17" t="s">
+      <c r="M17" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1440,7 +1462,7 @@
       <c r="L18" s="16">
         <v>0.82843999999999995</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1466,7 +1488,7 @@
         <v>58</v>
       </c>
       <c r="L19" s="16"/>
-      <c r="M19" t="s">
+      <c r="M19" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1496,7 +1518,7 @@
       <c r="L20" s="16">
         <v>0.82972999999999997</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1522,7 +1544,7 @@
         <v>47</v>
       </c>
       <c r="L21" s="16"/>
-      <c r="M21" t="s">
+      <c r="M21" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1552,7 +1574,7 @@
       <c r="L22" s="16">
         <v>0.83438000000000001</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1578,7 +1600,7 @@
         <v>47</v>
       </c>
       <c r="L23" s="16"/>
-      <c r="M23" t="s">
+      <c r="M23" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1608,7 +1630,7 @@
       <c r="L24" s="16">
         <v>0.83453999999999995</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1634,7 +1656,7 @@
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="16"/>
-      <c r="M25" t="s">
+      <c r="M25" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1660,7 +1682,7 @@
         <v>57</v>
       </c>
       <c r="L26" s="16"/>
-      <c r="M26" t="s">
+      <c r="M26" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1690,7 +1712,7 @@
       <c r="L27" s="16">
         <v>0.83076000000000005</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1716,7 +1738,7 @@
         <v>47</v>
       </c>
       <c r="L28" s="16"/>
-      <c r="M28" t="s">
+      <c r="M28" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1745,7 +1767,7 @@
       <c r="L29" s="17">
         <v>0.83511999999999997</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M29" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1773,7 +1795,7 @@
         <v>60</v>
       </c>
       <c r="L30" s="16"/>
-      <c r="M30" t="s">
+      <c r="M30" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1802,7 +1824,7 @@
       <c r="L31" s="16">
         <v>0.81272</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M31" s="16" t="s">
         <v>12</v>
       </c>
       <c r="N31" t="s">
@@ -1833,7 +1855,7 @@
         <v>0.9</v>
       </c>
       <c r="L32" s="16"/>
-      <c r="M32" t="s">
+      <c r="M32" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1861,7 +1883,7 @@
         <v>66</v>
       </c>
       <c r="L33" s="16"/>
-      <c r="M33" t="s">
+      <c r="M33" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1892,7 +1914,7 @@
         <v>0.90100000000000002</v>
       </c>
       <c r="L34" s="16"/>
-      <c r="M34" t="s">
+      <c r="M34" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1923,7 +1945,7 @@
         <v>0.89700000000000002</v>
       </c>
       <c r="L35" s="16"/>
-      <c r="M35" t="s">
+      <c r="M35" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1955,7 +1977,7 @@
       <c r="L36" s="16">
         <v>0.82679000000000002</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M36" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1984,7 +2006,7 @@
         <v>36</v>
       </c>
       <c r="L37" s="16"/>
-      <c r="M37" t="s">
+      <c r="M37" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2010,7 +2032,7 @@
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="16"/>
-      <c r="M38" t="s">
+      <c r="M38" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2036,7 +2058,7 @@
         <v>71</v>
       </c>
       <c r="L39" s="16"/>
-      <c r="M39" t="s">
+      <c r="M39" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2065,7 +2087,7 @@
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="16"/>
-      <c r="M40" t="s">
+      <c r="M40" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2092,9 +2114,10 @@
         <v>71</v>
       </c>
       <c r="L41" s="18"/>
-      <c r="M41" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="M41" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N41" s="9"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="22">
@@ -2123,9 +2146,10 @@
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="18"/>
-      <c r="M42" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="M42" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N42" s="9"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="21">
@@ -2152,9 +2176,10 @@
         <v>78</v>
       </c>
       <c r="L43" s="18"/>
-      <c r="M43" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="M43" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N43" s="9"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="21">
@@ -2183,9 +2208,10 @@
       </c>
       <c r="K44" s="13"/>
       <c r="L44" s="18"/>
-      <c r="M44" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="M44" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N44" s="9"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="21">
@@ -2214,9 +2240,10 @@
       </c>
       <c r="K45" s="13"/>
       <c r="L45" s="18"/>
-      <c r="M45" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="M45" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N45" s="9"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="21">
@@ -2247,7 +2274,7 @@
       <c r="L46" s="18">
         <v>0.82506999999999997</v>
       </c>
-      <c r="M46" s="9" t="s">
+      <c r="M46" s="18" t="s">
         <v>12</v>
       </c>
       <c r="N46" t="s">
@@ -2281,7 +2308,7 @@
         <v>83</v>
       </c>
       <c r="L47" s="16"/>
-      <c r="M47" t="s">
+      <c r="M47" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2312,11 +2339,11 @@
         <v>84</v>
       </c>
       <c r="L48" s="16"/>
-      <c r="M48" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M48" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="21">
         <v>44986.404861111114</v>
       </c>
@@ -2337,11 +2364,11 @@
         <v>85</v>
       </c>
       <c r="L49" s="16"/>
-      <c r="M49" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M49" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="21">
         <v>44986.406944444447</v>
       </c>
@@ -2365,11 +2392,11 @@
         <v>88</v>
       </c>
       <c r="L50" s="16"/>
-      <c r="M50" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M50" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="21">
         <v>44986.411805555559</v>
       </c>
@@ -2391,11 +2418,11 @@
         <v>89</v>
       </c>
       <c r="L51" s="16"/>
-      <c r="M51" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M51" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="21">
         <v>44986.430555555555</v>
       </c>
@@ -2417,11 +2444,11 @@
         <v>91</v>
       </c>
       <c r="L52" s="16"/>
-      <c r="M52" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M52" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="21">
         <v>44986.440972222219</v>
       </c>
@@ -2445,11 +2472,11 @@
         <v>91</v>
       </c>
       <c r="L53" s="16"/>
-      <c r="M53" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M53" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="21">
         <v>44986.440972222219</v>
       </c>
@@ -2473,11 +2500,11 @@
         <v>91</v>
       </c>
       <c r="L54" s="16"/>
-      <c r="M54" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M54" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="21">
         <v>44988.951388888891</v>
       </c>
@@ -2498,8 +2525,130 @@
         <v>0.85599999999999998</v>
       </c>
       <c r="L55" s="16"/>
-      <c r="M55" t="s">
+      <c r="M55" s="16" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" s="21">
+        <v>44991.878948032405</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" t="s">
+        <v>99</v>
+      </c>
+      <c r="G56" t="s">
+        <v>55</v>
+      </c>
+      <c r="I56" s="5">
+        <v>1</v>
+      </c>
+      <c r="J56" s="5">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" s="21">
+        <v>44991.882490162039</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" t="s">
+        <v>99</v>
+      </c>
+      <c r="G57" t="s">
+        <v>55</v>
+      </c>
+      <c r="I57" s="5">
+        <v>1</v>
+      </c>
+      <c r="L57" s="16">
+        <v>0.83465</v>
+      </c>
+      <c r="M57" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" s="21">
+        <v>44991.887632060185</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" t="s">
+        <v>99</v>
+      </c>
+      <c r="G58" t="s">
+        <v>55</v>
+      </c>
+      <c r="I58" s="5">
+        <v>1</v>
+      </c>
+      <c r="J58" s="5">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="L58" s="16"/>
+      <c r="M58" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" s="21">
+        <v>44991.889409027775</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" t="s">
+        <v>99</v>
+      </c>
+      <c r="G59" t="s">
+        <v>55</v>
+      </c>
+      <c r="I59" s="5">
+        <v>1</v>
+      </c>
+      <c r="L59" s="16">
+        <v>0.83423000000000003</v>
+      </c>
+      <c r="M59" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N59" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2522,13 +2671,13 @@
           <x14:formula1>
             <xm:f>Dropdowns!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>M38 M40 M42 M2:M36</xm:sqref>
+          <xm:sqref>N38 N40 N42 N3:N30 N32:N36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{82231E75-7DFD-C64F-B418-BB6F687712B9}">
           <x14:formula1>
             <xm:f>Dropdowns!$E:$E</xm:f>
           </x14:formula1>
-          <xm:sqref>D1 D56:D1048576 D2:D55</xm:sqref>
+          <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
fix comments on kaggle submissions
</commit_message>
<xml_diff>
--- a/modeling/modeling_tracker.xlsx
+++ b/modeling/modeling_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/Machine Learning II/ml2challenge/modeling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianna/Documents/master/2022-2023/Machine_learning_2/ml2challenge/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F34A8F-46AA-6346-8EF7-50FA6F73D227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84630586-1949-D64F-8CB3-1E76B0E0508B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{3C7B259C-6B95-FA44-938F-ACFA9CA61896}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="101">
   <si>
     <t>hyperparameters</t>
   </si>
@@ -322,46 +322,6 @@
   </si>
   <si>
     <t>pca_components</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Corpo)"/>
-      </rPr>
-      <t xml:space="preserve">!!! </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>In the submission  I did  said feat eng… the code was wrong, no feat eng, just pca on row data</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Corpo)"/>
-      </rPr>
-      <t xml:space="preserve">!!! </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> In the submission  I did  said feat eng… the code was wrong, no feat eng, just pca on row data</t>
-    </r>
   </si>
   <si>
     <t>Tuning Validation Acuuracy</t>
@@ -387,12 +347,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -426,11 +386,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Corpo)"/>
     </font>
   </fonts>
   <fills count="5">
@@ -507,7 +462,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -517,7 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -529,30 +484,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -561,28 +516,28 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Währung" xfId="1" builtinId="4"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Valuta" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.00000"/>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.00000"/>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -595,7 +550,7 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
+      <numFmt numFmtId="166" formatCode="d/m/yy\ h:mm;@"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -639,7 +594,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -938,8 +893,8 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="88" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+    <sheetView tabSelected="1" topLeftCell="G23" zoomScale="88" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -992,7 +947,7 @@
         <v>10</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>9</v>
@@ -1001,7 +956,7 @@
         <v>11</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1411,7 +1366,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="21">
         <v>44979.915972222225</v>
       </c>
@@ -1437,7 +1392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="21">
         <v>44979.930555555555</v>
       </c>
@@ -1466,7 +1421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="21">
         <v>44979.956944444442</v>
       </c>
@@ -1492,7 +1447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="21">
         <v>44979.959027777775</v>
       </c>
@@ -1522,7 +1477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="21">
         <v>44979.969444444447</v>
       </c>
@@ -1548,7 +1503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>44980.959027777775</v>
       </c>
@@ -1578,7 +1533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="21">
         <v>44979.376388888886</v>
       </c>
@@ -1604,7 +1559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="21">
         <v>44979.416666666664</v>
       </c>
@@ -1634,7 +1589,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="21">
         <v>44981.481944444444</v>
       </c>
@@ -1660,7 +1615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="21">
         <v>44981.506944444445</v>
       </c>
@@ -1686,7 +1641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="21">
         <v>44981.513194444444</v>
       </c>
@@ -1716,7 +1671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="21">
         <v>44981.51666666667</v>
       </c>
@@ -1742,7 +1697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="21">
         <v>44981.57916666667</v>
       </c>
@@ -1771,7 +1726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="21">
         <v>44985.458333333336</v>
       </c>
@@ -1799,7 +1754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="21">
         <v>44985.477777777778</v>
       </c>
@@ -1827,11 +1782,8 @@
       <c r="M31" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N31" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="21">
         <v>44985.513888888891</v>
       </c>
@@ -2277,9 +2229,6 @@
       <c r="M46" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="N46" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="21">
@@ -2513,7 +2462,7 @@
       </c>
       <c r="C55" s="1"/>
       <c r="D55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E55" t="s">
         <v>33</v>
@@ -2541,7 +2490,7 @@
         <v>15</v>
       </c>
       <c r="E56" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G56" t="s">
         <v>55</v>
@@ -2557,7 +2506,7 @@
         <v>14</v>
       </c>
       <c r="N56" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -2572,7 +2521,7 @@
         <v>15</v>
       </c>
       <c r="E57" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G57" t="s">
         <v>55</v>
@@ -2587,7 +2536,7 @@
         <v>14</v>
       </c>
       <c r="N57" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
@@ -2602,7 +2551,7 @@
         <v>15</v>
       </c>
       <c r="E58" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G58" t="s">
         <v>55</v>
@@ -2618,7 +2567,7 @@
         <v>14</v>
       </c>
       <c r="N58" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -2633,7 +2582,7 @@
         <v>15</v>
       </c>
       <c r="E59" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G59" t="s">
         <v>55</v>
@@ -2648,7 +2597,7 @@
         <v>14</v>
       </c>
       <c r="N59" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2772,7 +2721,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>